<commit_message>
Update 2. Example Tables v1.0 - 12Apr2019.xlsx
</commit_message>
<xml_diff>
--- a/Documents/2. Example Tables v1.0 - 12Apr2019.xlsx
+++ b/Documents/2. Example Tables v1.0 - 12Apr2019.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faith\Documents\Coding\Sky\Final Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faith\Documents\Coding\Sky\Final Project\TravelBlog\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AFAA09-4ED5-479B-8CCB-D17D3B8266FE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F728D671-4CA4-4741-BE3D-8B9D01A80C26}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="786" xr2:uid="{0DC0DBCC-9CB6-4DBE-A045-18AC3078640C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="786" activeTab="7" xr2:uid="{0DC0DBCC-9CB6-4DBE-A045-18AC3078640C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="7" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="131">
   <si>
     <t>CountryID</t>
   </si>
@@ -467,6 +467,18 @@
   </si>
   <si>
     <t>-DEFAULTS have been assigned in the "Blog" for "Likescounter"</t>
+  </si>
+  <si>
+    <t>Permission</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Location</t>
   </si>
 </sst>
 </file>
@@ -640,29 +652,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -678,6 +672,24 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -998,8 +1010,8 @@
   </sheetPr>
   <dimension ref="B2:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1009,194 +1021,194 @@
   <sheetData>
     <row r="2" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="2:15" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="5"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="23"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="8"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="5"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B5" s="9"/>
-      <c r="C5" s="10" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="8"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="5"/>
     </row>
     <row r="6" spans="2:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="9"/>
-      <c r="C6" s="11" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="17"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="11"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B7" s="9"/>
-      <c r="C7" s="10" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="8"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="5"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="8"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="5"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="12"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="26"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B10" s="13"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="12"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="26"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B11" s="9"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="8"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="5"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="20"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="14"/>
     </row>
     <row r="13" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="16"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1236,10 +1248,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5322720-99B8-40D5-90B4-C0976628FA32}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A14" sqref="A14:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1248,10 +1260,11 @@
     <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.81640625" customWidth="1"/>
-    <col min="5" max="6" width="8.7265625" style="1"/>
+    <col min="5" max="5" width="15.81640625" style="1" customWidth="1"/>
+    <col min="6" max="7" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1265,94 +1278,116 @@
         <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="15" t="s">
         <v>60</v>
       </c>
       <c r="B2" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="17" t="s">
         <v>68</v>
       </c>
       <c r="D2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="21" t="s">
+      <c r="E2" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="15" t="s">
         <v>61</v>
       </c>
       <c r="B3" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="17" t="s">
         <v>67</v>
       </c>
       <c r="D3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="21" t="s">
+      <c r="E3" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="15" t="s">
         <v>62</v>
       </c>
       <c r="B4" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="17" t="s">
         <v>70</v>
       </c>
       <c r="D4" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="21" t="s">
+      <c r="E4" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="15" t="s">
         <v>63</v>
       </c>
       <c r="B5" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="17" t="s">
         <v>72</v>
       </c>
       <c r="D5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="21" t="s">
+      <c r="E5" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="15" t="s">
         <v>64</v>
       </c>
       <c r="B6" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="17" t="s">
         <v>74</v>
       </c>
       <c r="D6" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E6" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E7" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>116</v>
       </c>
@@ -1413,7 +1448,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="15" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
@@ -1421,7 +1456,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B3" t="s">
@@ -1429,7 +1464,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B4" t="s">
@@ -1437,7 +1472,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
@@ -1445,7 +1480,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B6" t="s">
@@ -1453,7 +1488,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B7" t="s">
@@ -1461,7 +1496,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B8" t="s">
@@ -1469,7 +1504,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B9" t="s">
@@ -1477,7 +1512,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="15" t="s">
         <v>25</v>
       </c>
       <c r="B10" t="s">
@@ -1485,7 +1520,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="15" t="s">
         <v>26</v>
       </c>
       <c r="B11" t="s">
@@ -1493,7 +1528,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="15" t="s">
         <v>96</v>
       </c>
       <c r="B12" t="s">
@@ -1552,7 +1587,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="21">
+      <c r="A2" s="15">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -1560,7 +1595,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="21">
+      <c r="A3" s="15">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -1568,7 +1603,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="21">
+      <c r="A4" s="15">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -1576,7 +1611,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="21">
+      <c r="A5" s="15">
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -1584,7 +1619,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="21">
+      <c r="A6" s="15">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -1592,7 +1627,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="21">
+      <c r="A7" s="15">
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -1600,7 +1635,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="21">
+      <c r="A8" s="15">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -1608,7 +1643,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="21">
+      <c r="A9" s="15">
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -1643,7 +1678,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1661,7 +1696,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="21">
+      <c r="A2" s="15">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -1669,7 +1704,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="21">
+      <c r="A3" s="15">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -1677,7 +1712,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="21">
+      <c r="A4" s="15">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -1685,7 +1720,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="21">
+      <c r="A5" s="15">
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -1693,7 +1728,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="15" t="s">
         <v>86</v>
       </c>
       <c r="B6" t="s">
@@ -1701,13 +1736,13 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="21"/>
+      <c r="A7" s="15"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="21"/>
+      <c r="A8" s="15"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="21"/>
+      <c r="A9" s="15"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -1742,7 +1777,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:B17"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1750,7 +1785,7 @@
     <col min="1" max="1" width="27.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" style="22"/>
+    <col min="7" max="7" width="8.7265625" style="16"/>
     <col min="8" max="8" width="10.7265625" customWidth="1"/>
     <col min="9" max="9" width="12.81640625" customWidth="1"/>
     <col min="10" max="10" width="8.7265625" style="1"/>
@@ -1775,13 +1810,13 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="16" t="s">
         <v>57</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -1789,130 +1824,130 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="J2" s="26"/>
+      <c r="J2" s="20"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="J3" s="26"/>
+      <c r="J3" s="20"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="G4" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="I4" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="J4" s="26"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="26"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="20"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="26"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="20"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="26"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="E12" t="s">
@@ -1960,7 +1995,7 @@
       <c r="F16" t="s">
         <v>83</v>
       </c>
-      <c r="G16" s="22" t="s">
+      <c r="G16" s="16" t="s">
         <v>84</v>
       </c>
       <c r="H16" t="s">
@@ -2008,7 +2043,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057F2A7D-A17A-4280-B21B-54F997C79001}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
@@ -2019,39 +2054,51 @@
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>120</v>
       </c>
       <c r="B1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="C1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
         <v>121</v>
       </c>
-      <c r="B2" s="21" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>123</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="21" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -2059,24 +2106,33 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B16" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>82</v>
-      </c>
+      <c r="C16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>82</v>
       </c>
+      <c r="C17" t="s">
+        <v>82</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
@@ -2087,11 +2143,14 @@
   </sheetPr>
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.36328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>